<commit_message>
Interpreted undefined F1 measure as 0. Allowed generating LRR classifiers with single predictors. Searched for an optimal LRR classifier.
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5872210-E9F1-495F-9A31-65256079FFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF6FE8E-62CC-4514-8195-4EAD99D03253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22390" yWindow="50" windowWidth="15880" windowHeight="20850" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
+    <workbookView xWindow="16620" yWindow="50" windowWidth="21650" windowHeight="20850" activeTab="2" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Logistic_Regression" sheetId="1" r:id="rId1"/>
+    <sheet name="LR" sheetId="1" r:id="rId1"/>
+    <sheet name="LRR" sheetId="3" r:id="rId2"/>
+    <sheet name="LRR_From_Optimal_Two_Predictors" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
   <si>
     <t>Results Of Conducting Bidirectional Selection</t>
   </si>
@@ -33,9 +35,6 @@
     <t>Created: 08/07/2023 by Tom Lever</t>
   </si>
   <si>
-    <t>Updated: 08/07/2023 by Tom Lever</t>
-  </si>
-  <si>
     <t>Type Of Model</t>
   </si>
   <si>
@@ -187,6 +186,204 @@
   </si>
   <si>
     <t>Normalized_Square_Of_Red + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Logistic Ridge Regression</t>
+  </si>
+  <si>
+    <t>Updated: 08/08/2023 by Tom Lever</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Blue + Normalized_Interaction_Of_Green_And_Blue + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Green_And_Blue</t>
   </si>
 </sst>
 </file>
@@ -566,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34444DF7-7AEC-4A9B-9E91-22084E7B5E6A}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,26 +786,26 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>9.8000000000000004E-2</v>
@@ -616,7 +813,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>9.7000000000000003E-2</v>
@@ -624,7 +821,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>0.44500000000000001</v>
@@ -632,7 +829,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>9.0999999999999998E-2</v>
@@ -640,7 +837,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>9.7000000000000003E-2</v>
@@ -648,7 +845,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>0.44400000000000001</v>
@@ -656,7 +853,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>9.1999999999999998E-2</v>
@@ -664,7 +861,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>9.7000000000000003E-2</v>
@@ -672,7 +869,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>0.44500000000000001</v>
@@ -680,7 +877,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>8.8999999999999996E-2</v>
@@ -688,7 +885,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>8.7999999999999995E-2</v>
@@ -696,7 +893,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="3">
         <v>0.44600000000000001</v>
@@ -704,7 +901,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>9.7000000000000003E-2</v>
@@ -712,7 +909,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>0.44400000000000001</v>
@@ -720,7 +917,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23">
         <v>0.44400000000000001</v>
@@ -728,15 +925,15 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="4">
+        <v>21</v>
+      </c>
+      <c r="C25">
         <v>0.72099999999999997</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>0.66100000000000003</v>
@@ -744,7 +941,7 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27">
         <v>0.44600000000000001</v>
@@ -752,7 +949,7 @@
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28">
         <v>0.57799999999999996</v>
@@ -760,7 +957,7 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29">
         <v>0.54400000000000004</v>
@@ -768,7 +965,7 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30">
         <v>0.44600000000000001</v>
@@ -776,7 +973,7 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31">
         <v>0.64800000000000002</v>
@@ -784,7 +981,7 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32">
         <v>0.59</v>
@@ -792,7 +989,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33">
         <v>0.44600000000000001</v>
@@ -800,7 +997,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="3">
         <v>0.91200000000000003</v>
@@ -808,7 +1005,7 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35">
         <v>0.83499999999999996</v>
@@ -816,15 +1013,15 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
         <v>33</v>
-      </c>
-      <c r="C36" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37">
         <v>0.66200000000000003</v>
@@ -832,7 +1029,7 @@
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38">
         <v>0.44600000000000001</v>
@@ -840,7 +1037,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39">
         <v>0.44600000000000001</v>
@@ -848,15 +1045,15 @@
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="4">
+        <v>37</v>
+      </c>
+      <c r="C41">
         <v>0.93400000000000005</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42">
         <v>0.92900000000000005</v>
@@ -864,55 +1061,55 @@
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="4">
+        <v>39</v>
+      </c>
+      <c r="C43">
         <v>0.93400000000000005</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="4">
+        <v>40</v>
+      </c>
+      <c r="C44">
         <v>0.93600000000000005</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="4">
+        <v>41</v>
+      </c>
+      <c r="C45">
         <v>0.93400000000000005</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="4">
+        <v>42</v>
+      </c>
+      <c r="C46">
         <v>0.93700000000000006</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="4">
+        <v>43</v>
+      </c>
+      <c r="C47">
         <v>0.93600000000000005</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="4">
+        <v>44</v>
+      </c>
+      <c r="C48">
         <v>0.93200000000000005</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C49" s="3">
         <v>0.93700000000000006</v>
@@ -920,31 +1117,31 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="C50" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="4">
+        <v>47</v>
+      </c>
+      <c r="C51">
         <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C53">
         <v>0.92900000000000005</v>
@@ -952,7 +1149,7 @@
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54">
         <v>0.93400000000000005</v>
@@ -960,7 +1157,7 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55">
         <v>0.93400000000000005</v>
@@ -968,10 +1165,885 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57">
         <v>0.90300000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F19B04-EE74-45BF-A4B9-5BB8AF367F72}">
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.90625" customWidth="1"/>
+    <col min="2" max="2" width="105.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4">
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="4">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="4">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="4">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.44700000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.44700000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0.44700000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="4">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C56" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44352D9-B471-4505-836D-2A762E5E5452}">
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.90625" customWidth="1"/>
+    <col min="2" max="2" width="180.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.65300000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="4">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.63500000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B40" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B41" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.69199999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B56" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B58" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" s="4">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B59" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B60" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B62" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="4">
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Used Peter Gedeck's ranges of costs, degrees, and values of gamma. Conducted bidirectional selection for LDA, QDA, and KNN.
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF6FE8E-62CC-4514-8195-4EAD99D03253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC35D232-E8E5-4369-B53E-6C94298F6A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16620" yWindow="50" windowWidth="21650" windowHeight="20850" activeTab="2" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
+    <workbookView xWindow="23760" yWindow="50" windowWidth="14510" windowHeight="20850" activeTab="5" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
   </bookViews>
   <sheets>
     <sheet name="LR" sheetId="1" r:id="rId1"/>
     <sheet name="LRR" sheetId="3" r:id="rId2"/>
     <sheet name="LRR_From_Optimal_Two_Predictors" sheetId="4" r:id="rId3"/>
+    <sheet name="LDA" sheetId="5" r:id="rId4"/>
+    <sheet name="QDA" sheetId="6" r:id="rId5"/>
+    <sheet name="KNN" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="185">
   <si>
     <t>Results Of Conducting Bidirectional Selection</t>
   </si>
@@ -384,6 +387,204 @@
   </si>
   <si>
     <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Blue + Normalized_Square_Of_Red + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Updated: 08/09/2023 by Tom Lever</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t>QDA</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Interaction_Of_Green_And_Blue</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1380,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F19B04-EE74-45BF-A4B9-5BB8AF367F72}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
@@ -1225,7 +1426,7 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
@@ -1233,7 +1434,7 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
@@ -1241,7 +1442,7 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11">
         <v>0.44500000000000001</v>
       </c>
     </row>
@@ -1249,7 +1450,7 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12">
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
@@ -1257,7 +1458,7 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
@@ -1265,7 +1466,7 @@
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14">
         <v>0.44500000000000001</v>
       </c>
     </row>
@@ -1273,7 +1474,7 @@
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15">
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
@@ -1281,7 +1482,7 @@
       <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
@@ -1289,7 +1490,7 @@
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17">
         <v>0.44500000000000001</v>
       </c>
     </row>
@@ -1297,7 +1498,7 @@
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
@@ -1305,7 +1506,7 @@
       <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
@@ -1321,7 +1522,7 @@
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
@@ -1329,7 +1530,7 @@
       <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22">
         <v>0.442</v>
       </c>
     </row>
@@ -1337,18 +1538,15 @@
       <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23">
         <v>0.44400000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -1356,7 +1554,7 @@
       <c r="B26" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26">
         <v>0</v>
       </c>
     </row>
@@ -1364,7 +1562,7 @@
       <c r="B27" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27">
         <v>0.44500000000000001</v>
       </c>
     </row>
@@ -1372,7 +1570,7 @@
       <c r="B28" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28">
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
@@ -1380,7 +1578,7 @@
       <c r="B29" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29">
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
@@ -1388,7 +1586,7 @@
       <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30">
         <v>0.44600000000000001</v>
       </c>
     </row>
@@ -1396,7 +1594,7 @@
       <c r="B31" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31">
         <v>2.7E-2</v>
       </c>
     </row>
@@ -1404,7 +1602,7 @@
       <c r="B32" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32">
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
@@ -1412,7 +1610,7 @@
       <c r="B33" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33">
         <v>0.44600000000000001</v>
       </c>
     </row>
@@ -1420,7 +1618,7 @@
       <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
@@ -1428,7 +1626,7 @@
       <c r="B35" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1436,7 +1634,7 @@
       <c r="B36" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1444,7 +1642,7 @@
       <c r="B37" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37">
         <v>2.7E-2</v>
       </c>
     </row>
@@ -1452,7 +1650,7 @@
       <c r="B38" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38">
         <v>0.44700000000000001</v>
       </c>
     </row>
@@ -1464,14 +1662,11 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C40" s="4"/>
-    </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41">
         <v>1.2E-2</v>
       </c>
     </row>
@@ -1479,7 +1674,7 @@
       <c r="B42" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42">
         <v>0</v>
       </c>
     </row>
@@ -1487,7 +1682,7 @@
       <c r="B43" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43">
         <v>0.44600000000000001</v>
       </c>
     </row>
@@ -1495,7 +1690,7 @@
       <c r="B44" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1503,7 +1698,7 @@
       <c r="B45" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45">
         <v>1.2E-2</v>
       </c>
     </row>
@@ -1519,7 +1714,7 @@
       <c r="B47" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1527,7 +1722,7 @@
       <c r="B48" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1535,7 +1730,7 @@
       <c r="B49" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49">
         <v>0.44600000000000001</v>
       </c>
     </row>
@@ -1543,7 +1738,7 @@
       <c r="B50" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50">
         <v>1.2E-2</v>
       </c>
     </row>
@@ -1551,7 +1746,7 @@
       <c r="B51" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1559,7 +1754,7 @@
       <c r="B52" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1567,7 +1762,7 @@
       <c r="B53" t="s">
         <v>67</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53">
         <v>0</v>
       </c>
     </row>
@@ -1575,7 +1770,7 @@
       <c r="B54" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54">
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
@@ -1583,12 +1778,9 @@
       <c r="B55" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C56" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1600,7 +1792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44352D9-B471-4505-836D-2A762E5E5452}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1647,26 +1839,26 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11">
         <v>0.65300000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12">
         <v>0.93200000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1674,12 +1866,12 @@
       <c r="B14" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14">
         <v>0.93600000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>75</v>
       </c>
       <c r="C15" s="3">
@@ -1690,7 +1882,7 @@
       <c r="B16" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1698,7 +1890,7 @@
       <c r="B17" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1706,7 +1898,7 @@
       <c r="B18" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>0.93500000000000005</v>
       </c>
     </row>
@@ -1714,7 +1906,7 @@
       <c r="B19" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
@@ -1722,7 +1914,7 @@
       <c r="B20" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
         <v>0.91700000000000004</v>
       </c>
     </row>
@@ -1730,7 +1922,7 @@
       <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <v>0.93100000000000005</v>
       </c>
     </row>
@@ -1738,7 +1930,7 @@
       <c r="B22" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22">
         <v>0</v>
       </c>
     </row>
@@ -1746,7 +1938,7 @@
       <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23">
         <v>0.93200000000000005</v>
       </c>
     </row>
@@ -1754,7 +1946,7 @@
       <c r="B24" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1762,52 +1954,44 @@
       <c r="B25" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-    </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27">
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-    </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="4" t="s">
+      <c r="B29" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29">
         <v>0.63500000000000001</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="4" t="s">
+      <c r="B30" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30">
         <v>0.93500000000000005</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="4" t="s">
+      <c r="B31" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="4" t="s">
+      <c r="B32" t="s">
         <v>90</v>
       </c>
       <c r="C32" s="3">
@@ -1815,236 +1999,1497 @@
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="4" t="s">
+      <c r="B33" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B34" s="4" t="s">
+      <c r="B34" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B35" s="4" t="s">
+      <c r="B35" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s">
         <v>94</v>
       </c>
+      <c r="C36">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41">
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45">
+        <v>0.69199999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B860205E-E1FC-4AF2-BCA5-2F337716C2FB}">
+  <dimension ref="A1:C57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="91.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.439</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.441</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4">
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.443</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.67100000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.61699999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.44700000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.68700000000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>130</v>
+      </c>
       <c r="C36" s="4">
-        <v>0.93700000000000006</v>
+        <v>0.44600000000000001</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="4" t="s">
-        <v>95</v>
+      <c r="B37" t="s">
+        <v>131</v>
       </c>
       <c r="C37" s="4">
-        <v>6.0000000000000001E-3</v>
+        <v>0.752</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38" s="4" t="s">
-        <v>96</v>
+      <c r="B38" t="s">
+        <v>132</v>
       </c>
       <c r="C38" s="4">
-        <v>0.46300000000000002</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="4" t="s">
-        <v>97</v>
+      <c r="B39" t="s">
+        <v>133</v>
       </c>
       <c r="C39" s="4">
-        <v>0.93400000000000005</v>
+        <v>0.754</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="4">
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.86199999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.85899999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.86099999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.86299999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.86799999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0.86299999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B212AC66-1544-4FCE-ADF7-C01287B163F7}">
+  <dimension ref="A1:C57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="91.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.26200000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.25800000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.439</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.25800000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.443</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.441</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.443</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.77600000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.82199999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.74299999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.44700000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.90100000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.84199999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.78400000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="4"/>
+    </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" s="4" t="s">
-        <v>99</v>
+      <c r="B41" t="s">
+        <v>134</v>
       </c>
       <c r="C41" s="4">
-        <v>0.93500000000000005</v>
+        <v>0.91400000000000003</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="4" t="s">
-        <v>100</v>
+      <c r="B42" t="s">
+        <v>135</v>
       </c>
       <c r="C42" s="4">
+        <v>0.90700000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.90100000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2315BCA-BE68-41F1-B1B5-A704F37DD4B4}">
+  <dimension ref="A1:C57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.6328125" customWidth="1"/>
+    <col min="2" max="2" width="93.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.85599999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.94199999999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.90900000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.94099999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="4" t="s">
-        <v>101</v>
+      <c r="B43" t="s">
+        <v>172</v>
       </c>
       <c r="C43" s="4">
-        <v>1.2E-2</v>
+        <v>0.94399999999999995</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="B44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.94199999999999995</v>
+      </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45" s="4">
-        <v>0.69199999999999995</v>
+      <c r="B45" t="s">
+        <v>174</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.95699999999999996</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="4" t="s">
-        <v>103</v>
+      <c r="B46" t="s">
+        <v>175</v>
       </c>
       <c r="C46" s="4">
-        <v>0.92400000000000004</v>
+        <v>0.94399999999999995</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
+      <c r="B47" t="s">
+        <v>176</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.94299999999999995</v>
+      </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="4" t="s">
-        <v>104</v>
+      <c r="B48" t="s">
+        <v>177</v>
       </c>
       <c r="C48" s="4">
-        <v>0.189</v>
+        <v>0.95699999999999996</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49" s="4" t="s">
-        <v>105</v>
+      <c r="B49" t="s">
+        <v>178</v>
       </c>
       <c r="C49" s="4">
-        <v>0.65800000000000003</v>
+        <v>0.94499999999999995</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B50" s="4" t="s">
-        <v>106</v>
+      <c r="B50" t="s">
+        <v>179</v>
       </c>
       <c r="C50" s="4">
-        <v>0</v>
+        <v>0.94299999999999995</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B51" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>33</v>
+      <c r="B51" t="s">
+        <v>180</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.95399999999999996</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B52" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>33</v>
+      <c r="B52" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.94399999999999995</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>33</v>
+      <c r="B53" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.95599999999999996</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B54" s="4" t="s">
-        <v>110</v>
+      <c r="B54" t="s">
+        <v>183</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="3">
-        <v>0.93799999999999994</v>
+      <c r="B55" t="s">
+        <v>184</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.94299999999999995</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B56" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C56" s="4">
-        <v>0</v>
-      </c>
+      <c r="C56" s="4"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B57" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C57" s="4">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C58" s="4">
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B59" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B60" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="4">
-        <v>0.65800000000000003</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B61" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C61" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B62" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C62" s="4">
-        <v>6.0000000000000001E-3</v>
-      </c>
+      <c r="B57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added setting NA F1 measure to 0 to calculate_F1_measure. Moved toward automating bidirectional selection. Conducted bidirectional selection for random forests.
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC35D232-E8E5-4369-B53E-6C94298F6A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9AADEC-B45E-4F0D-874B-60508FC17BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23760" yWindow="50" windowWidth="14510" windowHeight="20850" activeTab="5" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
+    <workbookView xWindow="22300" yWindow="50" windowWidth="15970" windowHeight="20850" firstSheet="2" activeTab="6" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
   </bookViews>
   <sheets>
     <sheet name="LR" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="LDA" sheetId="5" r:id="rId4"/>
     <sheet name="QDA" sheetId="6" r:id="rId5"/>
     <sheet name="KNN" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="286">
   <si>
     <t>Results Of Conducting Bidirectional Selection</t>
   </si>
@@ -482,9 +483,6 @@
     <t>Updated: 08/09/2023 by Tom Lever</t>
   </si>
   <si>
-    <t>CONTINUE</t>
-  </si>
-  <si>
     <t>LDA</t>
   </si>
   <si>
@@ -585,6 +583,312 @@
   </si>
   <si>
     <t>Normalized_Interaction_Of_Red_And_Blue + Normalized_Red + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Red + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Of_Red + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Red + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Green + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Natural_Logarithm_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Natural_Logarithm_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Natural_Logarithm_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Root_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Root_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Root_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Of_Red</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Of_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Of_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Interaction_Of_Red_And_Green</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Interaction_Of_Red_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Interaction_Of_Green_And_Blue</t>
+  </si>
+  <si>
+    <t>Normalized_Interaction_Of_Green_And_Blue + Normalized_Green</t>
   </si>
 </sst>
 </file>
@@ -1792,7 +2096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44352D9-B471-4505-836D-2A762E5E5452}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2232,7 +2536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B860205E-E1FC-4AF2-BCA5-2F337716C2FB}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2269,12 +2575,12 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
@@ -2282,7 +2588,7 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
@@ -2298,7 +2604,7 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12">
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
@@ -2306,7 +2612,7 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
@@ -2314,7 +2620,7 @@
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14">
         <v>0.439</v>
       </c>
     </row>
@@ -2322,7 +2628,7 @@
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15">
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
@@ -2330,7 +2636,7 @@
       <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16">
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
@@ -2338,7 +2644,7 @@
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17">
         <v>0.441</v>
       </c>
     </row>
@@ -2346,7 +2652,7 @@
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
@@ -2354,7 +2660,7 @@
       <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
@@ -2362,7 +2668,7 @@
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
         <v>0.44600000000000001</v>
       </c>
     </row>
@@ -2370,7 +2676,7 @@
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
@@ -2378,7 +2684,7 @@
       <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22">
         <v>0.443</v>
       </c>
     </row>
@@ -2386,18 +2692,15 @@
       <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23">
         <v>0.44500000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25">
         <v>0.77100000000000002</v>
       </c>
     </row>
@@ -2405,7 +2708,7 @@
       <c r="B26" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26">
         <v>0.753</v>
       </c>
     </row>
@@ -2413,7 +2716,7 @@
       <c r="B27" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27">
         <v>0.44400000000000001</v>
       </c>
     </row>
@@ -2421,7 +2724,7 @@
       <c r="B28" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28">
         <v>0.67100000000000004</v>
       </c>
     </row>
@@ -2429,7 +2732,7 @@
       <c r="B29" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29">
         <v>0.61699999999999999</v>
       </c>
     </row>
@@ -2437,7 +2740,7 @@
       <c r="B30" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30">
         <v>0.44700000000000001</v>
       </c>
     </row>
@@ -2445,7 +2748,7 @@
       <c r="B31" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31">
         <v>0.71499999999999997</v>
       </c>
     </row>
@@ -2453,7 +2756,7 @@
       <c r="B32" t="s">
         <v>126</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32">
         <v>0.68700000000000006</v>
       </c>
     </row>
@@ -2461,7 +2764,7 @@
       <c r="B33" t="s">
         <v>127</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33">
         <v>0.44600000000000001</v>
       </c>
     </row>
@@ -2477,7 +2780,7 @@
       <c r="B35" t="s">
         <v>129</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35">
         <v>0.84399999999999997</v>
       </c>
     </row>
@@ -2485,7 +2788,7 @@
       <c r="B36" t="s">
         <v>130</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36">
         <v>0.44600000000000001</v>
       </c>
     </row>
@@ -2493,7 +2796,7 @@
       <c r="B37" t="s">
         <v>131</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37">
         <v>0.752</v>
       </c>
     </row>
@@ -2501,7 +2804,7 @@
       <c r="B38" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38">
         <v>0.77</v>
       </c>
     </row>
@@ -2509,18 +2812,15 @@
       <c r="B39" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39">
         <v>0.754</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C40" s="4"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41">
         <v>0.86199999999999999</v>
       </c>
     </row>
@@ -2528,7 +2828,7 @@
       <c r="B42" t="s">
         <v>135</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42">
         <v>0.85899999999999999</v>
       </c>
     </row>
@@ -2536,7 +2836,7 @@
       <c r="B43" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43">
         <v>0.88100000000000001</v>
       </c>
     </row>
@@ -2544,7 +2844,7 @@
       <c r="B44" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44">
         <v>0.86599999999999999</v>
       </c>
     </row>
@@ -2552,7 +2852,7 @@
       <c r="B45" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45">
         <v>0.86099999999999999</v>
       </c>
     </row>
@@ -2560,7 +2860,7 @@
       <c r="B46" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46">
         <v>0.87</v>
       </c>
     </row>
@@ -2568,7 +2868,7 @@
       <c r="B47" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47">
         <v>0.86299999999999999</v>
       </c>
     </row>
@@ -2576,7 +2876,7 @@
       <c r="B48" t="s">
         <v>141</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48">
         <v>0.85499999999999998</v>
       </c>
     </row>
@@ -2584,7 +2884,7 @@
       <c r="B49" t="s">
         <v>142</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49">
         <v>0.87</v>
       </c>
     </row>
@@ -2592,7 +2892,7 @@
       <c r="B50" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50">
         <v>0.88100000000000001</v>
       </c>
     </row>
@@ -2608,7 +2908,7 @@
       <c r="B52" t="s">
         <v>145</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52">
         <v>0.86799999999999999</v>
       </c>
     </row>
@@ -2616,7 +2916,7 @@
       <c r="B53" t="s">
         <v>146</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53">
         <v>0.86</v>
       </c>
     </row>
@@ -2624,7 +2924,7 @@
       <c r="B54" t="s">
         <v>147</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54">
         <v>0.86299999999999999</v>
       </c>
     </row>
@@ -2632,18 +2932,17 @@
       <c r="B55" t="s">
         <v>148</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C56" s="4"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>150</v>
-      </c>
-      <c r="C57" s="4"/>
+        <v>184</v>
+      </c>
+      <c r="C57">
+        <v>0.71699999999999997</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2655,7 +2954,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B212AC66-1544-4FCE-ADF7-C01287B163F7}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2692,12 +2993,12 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>0.26200000000000001</v>
       </c>
     </row>
@@ -2705,7 +3006,7 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>0.10299999999999999</v>
       </c>
     </row>
@@ -2721,7 +3022,7 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12">
         <v>0.25800000000000001</v>
       </c>
     </row>
@@ -2729,7 +3030,7 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13">
         <v>0.115</v>
       </c>
     </row>
@@ -2737,7 +3038,7 @@
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14">
         <v>0.439</v>
       </c>
     </row>
@@ -2745,7 +3046,7 @@
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15">
         <v>0.25800000000000001</v>
       </c>
     </row>
@@ -2753,7 +3054,7 @@
       <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16">
         <v>0.108</v>
       </c>
     </row>
@@ -2761,7 +3062,7 @@
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17">
         <v>0.443</v>
       </c>
     </row>
@@ -2769,7 +3070,7 @@
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>0.26400000000000001</v>
       </c>
     </row>
@@ -2777,7 +3078,7 @@
       <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>0.10299999999999999</v>
       </c>
     </row>
@@ -2785,7 +3086,7 @@
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
         <v>0.44600000000000001</v>
       </c>
     </row>
@@ -2793,7 +3094,7 @@
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <v>0.104</v>
       </c>
     </row>
@@ -2801,7 +3102,7 @@
       <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22">
         <v>0.441</v>
       </c>
     </row>
@@ -2809,18 +3110,15 @@
       <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23">
         <v>0.443</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25">
         <v>0.88900000000000001</v>
       </c>
     </row>
@@ -2828,7 +3126,7 @@
       <c r="B26" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26">
         <v>0.78500000000000003</v>
       </c>
     </row>
@@ -2836,7 +3134,7 @@
       <c r="B27" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27">
         <v>0.44400000000000001</v>
       </c>
     </row>
@@ -2844,7 +3142,7 @@
       <c r="B28" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28">
         <v>0.77600000000000002</v>
       </c>
     </row>
@@ -2852,7 +3150,7 @@
       <c r="B29" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29">
         <v>0.70799999999999996</v>
       </c>
     </row>
@@ -2860,7 +3158,7 @@
       <c r="B30" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30">
         <v>0.44500000000000001</v>
       </c>
     </row>
@@ -2868,7 +3166,7 @@
       <c r="B31" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31">
         <v>0.82199999999999995</v>
       </c>
     </row>
@@ -2876,7 +3174,7 @@
       <c r="B32" t="s">
         <v>126</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32">
         <v>0.74299999999999999</v>
       </c>
     </row>
@@ -2884,7 +3182,7 @@
       <c r="B33" t="s">
         <v>127</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33">
         <v>0.44700000000000001</v>
       </c>
     </row>
@@ -2900,7 +3198,7 @@
       <c r="B35" t="s">
         <v>129</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35">
         <v>0.84199999999999997</v>
       </c>
     </row>
@@ -2908,7 +3206,7 @@
       <c r="B36" t="s">
         <v>130</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36">
         <v>0.44600000000000001</v>
       </c>
     </row>
@@ -2916,7 +3214,7 @@
       <c r="B37" t="s">
         <v>131</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37">
         <v>0.78400000000000003</v>
       </c>
     </row>
@@ -2924,7 +3222,7 @@
       <c r="B38" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38">
         <v>0.88800000000000001</v>
       </c>
     </row>
@@ -2932,18 +3230,15 @@
       <c r="B39" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39">
         <v>0.78600000000000003</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C40" s="4"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41">
         <v>0.91400000000000003</v>
       </c>
     </row>
@@ -2951,7 +3246,7 @@
       <c r="B42" t="s">
         <v>135</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42">
         <v>0.90700000000000003</v>
       </c>
     </row>
@@ -2959,7 +3254,7 @@
       <c r="B43" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43">
         <v>0.9</v>
       </c>
     </row>
@@ -2967,7 +3262,7 @@
       <c r="B44" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44">
         <v>0.91300000000000003</v>
       </c>
     </row>
@@ -2975,7 +3270,7 @@
       <c r="B45" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45">
         <v>0.91100000000000003</v>
       </c>
     </row>
@@ -2983,7 +3278,7 @@
       <c r="B46" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46">
         <v>0.90100000000000002</v>
       </c>
     </row>
@@ -2991,7 +3286,7 @@
       <c r="B47" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47">
         <v>0.91300000000000003</v>
       </c>
     </row>
@@ -2999,7 +3294,7 @@
       <c r="B48" t="s">
         <v>141</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48">
         <v>0.91</v>
       </c>
     </row>
@@ -3007,7 +3302,7 @@
       <c r="B49" t="s">
         <v>142</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49">
         <v>0.89</v>
       </c>
     </row>
@@ -3015,7 +3310,7 @@
       <c r="B50" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50">
         <v>0.9</v>
       </c>
     </row>
@@ -3023,7 +3318,7 @@
       <c r="B51" t="s">
         <v>144</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51">
         <v>0.90600000000000003</v>
       </c>
     </row>
@@ -3031,7 +3326,7 @@
       <c r="B52" t="s">
         <v>145</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52">
         <v>0.82599999999999996</v>
       </c>
     </row>
@@ -3039,7 +3334,7 @@
       <c r="B53" t="s">
         <v>146</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53">
         <v>0.90600000000000003</v>
       </c>
     </row>
@@ -3055,18 +3350,17 @@
       <c r="B55" t="s">
         <v>148</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55">
         <v>0.90600000000000003</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C56" s="4"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>150</v>
-      </c>
-      <c r="C57" s="4"/>
+        <v>185</v>
+      </c>
+      <c r="C57">
+        <v>0.9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3078,7 +3372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2315BCA-BE68-41F1-B1B5-A704F37DD4B4}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3115,109 +3411,109 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>154</v>
+      <c r="C9" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>154</v>
+      <c r="C10" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>154</v>
+      <c r="C11" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>154</v>
+      <c r="C12" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>154</v>
+      <c r="C13" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>154</v>
+      <c r="C14" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>154</v>
+      <c r="C15" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>154</v>
+      <c r="C16" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>154</v>
+      <c r="C17" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>154</v>
+      <c r="C18" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>154</v>
+      <c r="C19" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>154</v>
+      <c r="C20" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>154</v>
+      <c r="C21" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
@@ -3232,16 +3528,13 @@
       <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23">
         <v>0.85599999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C25" s="3">
         <v>0.94399999999999995</v>
@@ -3249,154 +3542,151 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>156</v>
-      </c>
-      <c r="C26" s="4">
+        <v>155</v>
+      </c>
+      <c r="C26">
         <v>0.90800000000000003</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>157</v>
-      </c>
-      <c r="C27" s="4">
+        <v>156</v>
+      </c>
+      <c r="C27">
         <v>0.92900000000000005</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="4">
+        <v>157</v>
+      </c>
+      <c r="C28">
         <v>0.94299999999999995</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>159</v>
-      </c>
-      <c r="C29" s="4">
+        <v>158</v>
+      </c>
+      <c r="C29">
         <v>0.91</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>160</v>
-      </c>
-      <c r="C30" s="4">
+        <v>159</v>
+      </c>
+      <c r="C30">
         <v>0.92800000000000005</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>161</v>
-      </c>
-      <c r="C31" s="4">
+        <v>160</v>
+      </c>
+      <c r="C31">
         <v>0.94299999999999995</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>162</v>
-      </c>
-      <c r="C32" s="4">
+        <v>161</v>
+      </c>
+      <c r="C32">
         <v>0.91100000000000003</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>163</v>
-      </c>
-      <c r="C33" s="4">
+        <v>162</v>
+      </c>
+      <c r="C33">
         <v>0.93100000000000005</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>164</v>
-      </c>
-      <c r="C34" s="4">
+        <v>163</v>
+      </c>
+      <c r="C34">
         <v>0.94199999999999995</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>165</v>
-      </c>
-      <c r="C35" s="4">
+        <v>164</v>
+      </c>
+      <c r="C35">
         <v>0.90900000000000003</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>166</v>
-      </c>
-      <c r="C36" s="4">
+        <v>165</v>
+      </c>
+      <c r="C36">
         <v>0.93</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>167</v>
-      </c>
-      <c r="C37" s="4">
+        <v>166</v>
+      </c>
+      <c r="C37">
         <v>0.91</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>168</v>
-      </c>
-      <c r="C38" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>169</v>
-      </c>
-      <c r="C39" s="4">
+        <v>168</v>
+      </c>
+      <c r="C39">
         <v>0.94099999999999995</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C40" s="4"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>170</v>
-      </c>
-      <c r="C41" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>171</v>
-      </c>
-      <c r="C42" s="4">
+        <v>170</v>
+      </c>
+      <c r="C42">
         <v>0.95599999999999996</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>172</v>
-      </c>
-      <c r="C43" s="4">
+        <v>171</v>
+      </c>
+      <c r="C43">
         <v>0.94399999999999995</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>173</v>
-      </c>
-      <c r="C44" s="4">
+        <v>172</v>
+      </c>
+      <c r="C44">
         <v>0.94199999999999995</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C45" s="3">
         <v>0.95699999999999996</v>
@@ -3404,95 +3694,1123 @@
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>175</v>
-      </c>
-      <c r="C46" s="4">
+        <v>174</v>
+      </c>
+      <c r="C46">
         <v>0.94399999999999995</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>176</v>
-      </c>
-      <c r="C47" s="4">
+        <v>175</v>
+      </c>
+      <c r="C47">
         <v>0.94299999999999995</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>177</v>
-      </c>
-      <c r="C48" s="4">
+        <v>176</v>
+      </c>
+      <c r="C48">
         <v>0.95699999999999996</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>178</v>
-      </c>
-      <c r="C49" s="4">
+        <v>177</v>
+      </c>
+      <c r="C49">
         <v>0.94499999999999995</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>179</v>
-      </c>
-      <c r="C50" s="4">
+        <v>178</v>
+      </c>
+      <c r="C50">
         <v>0.94299999999999995</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>180</v>
-      </c>
-      <c r="C51" s="4">
+        <v>179</v>
+      </c>
+      <c r="C51">
         <v>0.95399999999999996</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>181</v>
-      </c>
-      <c r="C52" s="4">
+        <v>180</v>
+      </c>
+      <c r="C52">
         <v>0.94399999999999995</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>182</v>
-      </c>
-      <c r="C53" s="4">
+        <v>181</v>
+      </c>
+      <c r="C53">
         <v>0.95599999999999996</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>183</v>
-      </c>
-      <c r="C54" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>184</v>
-      </c>
-      <c r="C55" s="4">
+        <v>183</v>
+      </c>
+      <c r="C55">
         <v>0.94299999999999995</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C56" s="4"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>150</v>
-      </c>
-      <c r="C57" s="4"/>
+        <v>186</v>
+      </c>
+      <c r="C57" t="s">
+        <v>153</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AD0FE6-A9A8-4556-AB61-CC98B21626F8}">
+  <dimension ref="A1:C145"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.6328125" customWidth="1"/>
+    <col min="2" max="2" width="110.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.82899999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>197</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.82799999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>198</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.872</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.82399999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>206</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>207</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.86299999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>209</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>210</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.86799999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>211</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>212</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.86499999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>214</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>215</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>216</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.85899999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.86799999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.86799999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.85799999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.38200000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0.93100000000000005</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.38200000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.91600000000000004</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0.92700000000000005</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>217</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>218</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0.82899999999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>219</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>221</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0.82399999999999995</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>222</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>223</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>224</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B65" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C65" s="3">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>226</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>227</v>
+      </c>
+      <c r="C67" s="4">
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>228</v>
+      </c>
+      <c r="C68" s="4">
+        <v>0.91600000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>229</v>
+      </c>
+      <c r="C69" s="4">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>230</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>231</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0.94099999999999995</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>232</v>
+      </c>
+      <c r="C73" s="4">
+        <v>0.81799999999999995</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>233</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>234</v>
+      </c>
+      <c r="C75" s="4">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>235</v>
+      </c>
+      <c r="C76" s="4">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>236</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>237</v>
+      </c>
+      <c r="C78" s="4">
+        <v>0.86499999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>238</v>
+      </c>
+      <c r="C79" s="4">
+        <v>0.81899999999999995</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>239</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
+        <v>240</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0.58399999999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>241</v>
+      </c>
+      <c r="C82" s="4">
+        <v>0.79800000000000004</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>243</v>
+      </c>
+      <c r="C84" s="4">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
+        <v>244</v>
+      </c>
+      <c r="C85" s="4">
+        <v>0.81699999999999995</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>245</v>
+      </c>
+      <c r="C86" s="3">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B87" t="s">
+        <v>246</v>
+      </c>
+      <c r="C87" s="4">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>247</v>
+      </c>
+      <c r="C89" s="4">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>248</v>
+      </c>
+      <c r="C90" s="4">
+        <v>0.86799999999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B91" t="s">
+        <v>249</v>
+      </c>
+      <c r="C91" s="4">
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B92" t="s">
+        <v>250</v>
+      </c>
+      <c r="C92" s="3">
+        <v>0.93899999999999995</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B93" t="s">
+        <v>251</v>
+      </c>
+      <c r="C93" s="4">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
+        <v>252</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B95" t="s">
+        <v>70</v>
+      </c>
+      <c r="C95" s="4">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B96" t="s">
+        <v>253</v>
+      </c>
+      <c r="C96" s="4">
+        <v>0.86199999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B97" t="s">
+        <v>254</v>
+      </c>
+      <c r="C97" s="4">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B98" t="s">
+        <v>80</v>
+      </c>
+      <c r="C98" s="4">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B99" t="s">
+        <v>81</v>
+      </c>
+      <c r="C99" s="4">
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B100" t="s">
+        <v>255</v>
+      </c>
+      <c r="C100" s="4">
+        <v>0.38100000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
+        <v>83</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0.90100000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B102" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102" s="4">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B103" t="s">
+        <v>85</v>
+      </c>
+      <c r="C103" s="4">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B105" t="s">
+        <v>256</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B106" t="s">
+        <v>257</v>
+      </c>
+      <c r="C106" s="4">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B107" t="s">
+        <v>258</v>
+      </c>
+      <c r="C107" s="4">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B108" t="s">
+        <v>259</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B109" t="s">
+        <v>86</v>
+      </c>
+      <c r="C109" s="4">
+        <v>0.82399999999999995</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B110" t="s">
+        <v>260</v>
+      </c>
+      <c r="C110" s="4">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B111" t="s">
+        <v>261</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B112" t="s">
+        <v>262</v>
+      </c>
+      <c r="C112" s="4">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B113" t="s">
+        <v>263</v>
+      </c>
+      <c r="C113" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B114" t="s">
+        <v>264</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B115" t="s">
+        <v>265</v>
+      </c>
+      <c r="C115" s="4">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B116" t="s">
+        <v>266</v>
+      </c>
+      <c r="C116" s="4">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B117" t="s">
+        <v>267</v>
+      </c>
+      <c r="C117" s="4">
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B118" t="s">
+        <v>268</v>
+      </c>
+      <c r="C118" s="4">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B119" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C119" s="4">
+        <v>0.94127620000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B129" t="s">
+        <v>270</v>
+      </c>
+      <c r="C129">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B130" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C130" s="3">
+        <v>0.95473439999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B131" t="s">
+        <v>272</v>
+      </c>
+      <c r="C131">
+        <v>0.94099999999999995</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B132" t="s">
+        <v>273</v>
+      </c>
+      <c r="C132">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B133" t="s">
+        <v>274</v>
+      </c>
+      <c r="C133">
+        <v>0.95399999999999996</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B134" t="s">
+        <v>275</v>
+      </c>
+      <c r="C134">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B135" t="s">
+        <v>276</v>
+      </c>
+      <c r="C135">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B136" t="s">
+        <v>277</v>
+      </c>
+      <c r="C136">
+        <v>0.95399999999999996</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B137" t="s">
+        <v>278</v>
+      </c>
+      <c r="C137">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B138" t="s">
+        <v>279</v>
+      </c>
+      <c r="C138">
+        <v>0.93899999999999995</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B139" t="s">
+        <v>280</v>
+      </c>
+      <c r="C139">
+        <v>0.95399999999999996</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B140" t="s">
+        <v>281</v>
+      </c>
+      <c r="C140">
+        <v>0.94099999999999995</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B141" t="s">
+        <v>282</v>
+      </c>
+      <c r="C141">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B142" t="s">
+        <v>283</v>
+      </c>
+      <c r="C142">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B143" t="s">
+        <v>284</v>
+      </c>
+      <c r="C143">
+        <v>0.94199999999999995</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B145" t="s">
+        <v>285</v>
+      </c>
+      <c r="C145">
+        <v>0.86799999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed formulas. Summarized performance of cross validated LDA's.
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9AADEC-B45E-4F0D-874B-60508FC17BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF4B996-9253-4826-B657-6479142D2D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22300" yWindow="50" windowWidth="15970" windowHeight="20850" firstSheet="2" activeTab="6" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
+    <workbookView xWindow="16270" yWindow="50" windowWidth="22000" windowHeight="20850" activeTab="3" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
   </bookViews>
   <sheets>
     <sheet name="LR" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="LDA" sheetId="5" r:id="rId4"/>
     <sheet name="QDA" sheetId="6" r:id="rId5"/>
     <sheet name="KNN" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="187">
   <si>
     <t>Results Of Conducting Bidirectional Selection</t>
   </si>
@@ -592,303 +591,6 @@
   </si>
   <si>
     <t>Normalized_Red + Normalized_Natural_Logarithm_Of_Green</t>
-  </si>
-  <si>
-    <t>Random Forest</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Natural_Logarithm_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Natural_Logarithm_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Square_Root_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Square_Root_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Square_Root_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Square_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Square_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Square_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Interaction_Of_Red_And_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Interaction_Of_Red_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Red + Normalized_Interaction_Of_Green_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Natural_Logarithm_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Natural_Logarithm_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Natural_Logarithm_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Square_Root_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Square_Root_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Square_Root_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Square_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Square_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Square_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Interaction_Of_Red_And_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Interaction_Of_Red_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Green + Normalized_Interaction_Of_Green_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Natural_Logarithm_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Natural_Logarithm_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Natural_Logarithm_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Root_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Root_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Root_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Square_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Interaction_Of_Red_And_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Interaction_Of_Red_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Red + Normalized_Interaction_Of_Green_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Natural_Logarithm_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Root_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Root_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Root_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Square_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Interaction_Of_Red_And_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Interaction_Of_Red_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Green + Normalized_Interaction_Of_Green_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Natural_Logarithm_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Natural_Logarithm_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Natural_Logarithm_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Root_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Natural_Logarithm_Of_Blue + Normalized_Square_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Natural_Logarithm_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Root_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Root_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Root_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Square_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Red_And_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Red_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Natural_Logarithm_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Natural_Logarithm_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Natural_Logarithm_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Root_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Root_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Root_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Of_Red</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Of_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Square_Of_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Interaction_Of_Red_And_Green</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Interaction_Of_Red_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Square_Root_Of_Red + Normalized_Interaction_Of_Green_And_Blue + Normalized_Interaction_Of_Green_And_Blue</t>
-  </si>
-  <si>
-    <t>Normalized_Interaction_Of_Green_And_Blue + Normalized_Green</t>
   </si>
 </sst>
 </file>
@@ -946,12 +648,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1268,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34444DF7-7AEC-4A9B-9E91-22084E7B5E6A}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2096,7 +1797,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44352D9-B471-4505-836D-2A762E5E5452}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2536,8 +2239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B860205E-E1FC-4AF2-BCA5-2F337716C2FB}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3373,7 +3076,7 @@
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3784,1033 +3487,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AD0FE6-A9A8-4556-AB61-CC98B21626F8}">
-  <dimension ref="A1:C145"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.6328125" customWidth="1"/>
-    <col min="2" max="2" width="110.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" t="s">
-        <v>189</v>
-      </c>
-      <c r="C9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C10">
-        <v>0.82599999999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>190</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>186</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0.82599999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>192</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>193</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>194</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.82899999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>195</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>196</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>197</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0.82799999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>198</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>199</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0.82299999999999995</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>200</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.93500000000000005</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
-        <v>201</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0.93600000000000005</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
-        <v>202</v>
-      </c>
-      <c r="C25" s="4">
-        <v>0.82299999999999995</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
-        <v>203</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>204</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0.872</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>205</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0.82399999999999995</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
-        <v>206</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>207</v>
-      </c>
-      <c r="C30" s="4">
-        <v>0.86299999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
-        <v>208</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0.82599999999999996</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>209</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
-        <v>210</v>
-      </c>
-      <c r="C33" s="4">
-        <v>0.86799999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>211</v>
-      </c>
-      <c r="C34" s="4">
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>212</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
-        <v>213</v>
-      </c>
-      <c r="C36" s="4">
-        <v>0.86499999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
-        <v>214</v>
-      </c>
-      <c r="C37" s="4">
-        <v>0.82099999999999995</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>215</v>
-      </c>
-      <c r="C38" s="3">
-        <v>0.90600000000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>216</v>
-      </c>
-      <c r="C39" s="4">
-        <v>0.85899999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" s="4">
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" s="4">
-        <v>0.86799999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="3">
-        <v>0.93700000000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="4">
-        <v>0.86799999999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" s="4">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="4">
-        <v>0.93200000000000005</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
-        <v>126</v>
-      </c>
-      <c r="C48" s="4">
-        <v>0.85799999999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" s="4">
-        <v>0.38200000000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B50" t="s">
-        <v>128</v>
-      </c>
-      <c r="C50" s="4">
-        <v>0.93100000000000005</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B51" t="s">
-        <v>129</v>
-      </c>
-      <c r="C51" s="4">
-        <v>0.86699999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B52" t="s">
-        <v>130</v>
-      </c>
-      <c r="C52" s="4">
-        <v>0.38200000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
-        <v>131</v>
-      </c>
-      <c r="C53" s="4">
-        <v>0.91600000000000004</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
-        <v>132</v>
-      </c>
-      <c r="C54" s="4">
-        <v>0.92700000000000005</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B55" t="s">
-        <v>133</v>
-      </c>
-      <c r="C55" s="4">
-        <v>0.84399999999999997</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B57" t="s">
-        <v>217</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B58" t="s">
-        <v>218</v>
-      </c>
-      <c r="C58" s="4">
-        <v>0.82899999999999996</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B59" t="s">
-        <v>219</v>
-      </c>
-      <c r="C59" s="4">
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B60" t="s">
-        <v>220</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B61" t="s">
-        <v>221</v>
-      </c>
-      <c r="C61" s="4">
-        <v>0.82399999999999995</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B62" t="s">
-        <v>222</v>
-      </c>
-      <c r="C62" s="4">
-        <v>0.93799999999999994</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B63" t="s">
-        <v>223</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
-        <v>224</v>
-      </c>
-      <c r="C64" s="4">
-        <v>0.82599999999999996</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B65" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C65" s="3">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B66" t="s">
-        <v>226</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B67" t="s">
-        <v>227</v>
-      </c>
-      <c r="C67" s="4">
-        <v>0.81499999999999995</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B68" t="s">
-        <v>228</v>
-      </c>
-      <c r="C68" s="4">
-        <v>0.91600000000000004</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B69" t="s">
-        <v>229</v>
-      </c>
-      <c r="C69" s="4">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B70" t="s">
-        <v>230</v>
-      </c>
-      <c r="C70" s="4">
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B71" t="s">
-        <v>231</v>
-      </c>
-      <c r="C71" s="4">
-        <v>0.94099999999999995</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B73" t="s">
-        <v>232</v>
-      </c>
-      <c r="C73" s="4">
-        <v>0.81799999999999995</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B74" t="s">
-        <v>233</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B75" t="s">
-        <v>234</v>
-      </c>
-      <c r="C75" s="4">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B76" t="s">
-        <v>235</v>
-      </c>
-      <c r="C76" s="4">
-        <v>0.82299999999999995</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B77" t="s">
-        <v>236</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B78" t="s">
-        <v>237</v>
-      </c>
-      <c r="C78" s="4">
-        <v>0.86499999999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B79" t="s">
-        <v>238</v>
-      </c>
-      <c r="C79" s="4">
-        <v>0.81899999999999995</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B80" t="s">
-        <v>239</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B81" t="s">
-        <v>240</v>
-      </c>
-      <c r="C81" s="4">
-        <v>0.58399999999999996</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B82" t="s">
-        <v>241</v>
-      </c>
-      <c r="C82" s="4">
-        <v>0.79800000000000004</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B83" t="s">
-        <v>242</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B84" t="s">
-        <v>243</v>
-      </c>
-      <c r="C84" s="4">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B85" t="s">
-        <v>244</v>
-      </c>
-      <c r="C85" s="4">
-        <v>0.81699999999999995</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B86" t="s">
-        <v>245</v>
-      </c>
-      <c r="C86" s="3">
-        <v>0.91200000000000003</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B87" t="s">
-        <v>246</v>
-      </c>
-      <c r="C87" s="4">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B89" t="s">
-        <v>247</v>
-      </c>
-      <c r="C89" s="4">
-        <v>0.92300000000000004</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B90" t="s">
-        <v>248</v>
-      </c>
-      <c r="C90" s="4">
-        <v>0.86799999999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B91" t="s">
-        <v>249</v>
-      </c>
-      <c r="C91" s="4">
-        <v>0.379</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B92" t="s">
-        <v>250</v>
-      </c>
-      <c r="C92" s="3">
-        <v>0.93899999999999995</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B93" t="s">
-        <v>251</v>
-      </c>
-      <c r="C93" s="4">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B94" t="s">
-        <v>252</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B95" t="s">
-        <v>70</v>
-      </c>
-      <c r="C95" s="4">
-        <v>0.93799999999999994</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B96" t="s">
-        <v>253</v>
-      </c>
-      <c r="C96" s="4">
-        <v>0.86199999999999999</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B97" t="s">
-        <v>254</v>
-      </c>
-      <c r="C97" s="4">
-        <v>0.40699999999999997</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B98" t="s">
-        <v>80</v>
-      </c>
-      <c r="C98" s="4">
-        <v>0.93600000000000005</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B99" t="s">
-        <v>81</v>
-      </c>
-      <c r="C99" s="4">
-        <v>0.86899999999999999</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B100" t="s">
-        <v>255</v>
-      </c>
-      <c r="C100" s="4">
-        <v>0.38100000000000001</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B101" t="s">
-        <v>83</v>
-      </c>
-      <c r="C101" s="4">
-        <v>0.90100000000000002</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B102" t="s">
-        <v>84</v>
-      </c>
-      <c r="C102" s="4">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B103" t="s">
-        <v>85</v>
-      </c>
-      <c r="C103" s="4">
-        <v>0.84399999999999997</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B105" t="s">
-        <v>256</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B106" t="s">
-        <v>257</v>
-      </c>
-      <c r="C106" s="4">
-        <v>0.82699999999999996</v>
-      </c>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B107" t="s">
-        <v>258</v>
-      </c>
-      <c r="C107" s="4">
-        <v>0.93799999999999994</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B108" t="s">
-        <v>259</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B109" t="s">
-        <v>86</v>
-      </c>
-      <c r="C109" s="4">
-        <v>0.82399999999999995</v>
-      </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B110" t="s">
-        <v>260</v>
-      </c>
-      <c r="C110" s="4">
-        <v>0.93300000000000005</v>
-      </c>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B111" t="s">
-        <v>261</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B112" t="s">
-        <v>262</v>
-      </c>
-      <c r="C112" s="4">
-        <v>0.81599999999999995</v>
-      </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B113" t="s">
-        <v>263</v>
-      </c>
-      <c r="C113" s="4">
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B114" t="s">
-        <v>264</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B115" t="s">
-        <v>265</v>
-      </c>
-      <c r="C115" s="4">
-        <v>0.82599999999999996</v>
-      </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B116" t="s">
-        <v>266</v>
-      </c>
-      <c r="C116" s="4">
-        <v>0.93300000000000005</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B117" t="s">
-        <v>267</v>
-      </c>
-      <c r="C117" s="4">
-        <v>0.81499999999999995</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B118" t="s">
-        <v>268</v>
-      </c>
-      <c r="C118" s="4">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B119" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="C119" s="4">
-        <v>0.94127620000000001</v>
-      </c>
-    </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B129" t="s">
-        <v>270</v>
-      </c>
-      <c r="C129">
-        <v>0.93799999999999994</v>
-      </c>
-    </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B130" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C130" s="3">
-        <v>0.95473439999999998</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B131" t="s">
-        <v>272</v>
-      </c>
-      <c r="C131">
-        <v>0.94099999999999995</v>
-      </c>
-    </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B132" t="s">
-        <v>273</v>
-      </c>
-      <c r="C132">
-        <v>0.93700000000000006</v>
-      </c>
-    </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B133" t="s">
-        <v>274</v>
-      </c>
-      <c r="C133">
-        <v>0.95399999999999996</v>
-      </c>
-    </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B134" t="s">
-        <v>275</v>
-      </c>
-      <c r="C134">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B135" t="s">
-        <v>276</v>
-      </c>
-      <c r="C135">
-        <v>0.93600000000000005</v>
-      </c>
-    </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B136" t="s">
-        <v>277</v>
-      </c>
-      <c r="C136">
-        <v>0.95399999999999996</v>
-      </c>
-    </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B137" t="s">
-        <v>278</v>
-      </c>
-      <c r="C137">
-        <v>0.93200000000000005</v>
-      </c>
-    </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B138" t="s">
-        <v>279</v>
-      </c>
-      <c r="C138">
-        <v>0.93899999999999995</v>
-      </c>
-    </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B139" t="s">
-        <v>280</v>
-      </c>
-      <c r="C139">
-        <v>0.95399999999999996</v>
-      </c>
-    </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B140" t="s">
-        <v>281</v>
-      </c>
-      <c r="C140">
-        <v>0.94099999999999995</v>
-      </c>
-    </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B141" t="s">
-        <v>282</v>
-      </c>
-      <c r="C141">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B142" t="s">
-        <v>283</v>
-      </c>
-      <c r="C142">
-        <v>0.93600000000000005</v>
-      </c>
-    </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B143" t="s">
-        <v>284</v>
-      </c>
-      <c r="C143">
-        <v>0.94199999999999995</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B145" t="s">
-        <v>285</v>
-      </c>
-      <c r="C145">
-        <v>0.86799999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Reconstructed images of regions 57, 67, 69, and 78. Summarized performance of cross validated QDA's.
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Results_Of_Conducting_Bidirectional_Selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF4B996-9253-4826-B657-6479142D2D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BE42C8-95A0-4640-AEC2-5FD2FAF9FA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16270" yWindow="50" windowWidth="22000" windowHeight="20850" activeTab="3" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
+    <workbookView xWindow="468" yWindow="192" windowWidth="21600" windowHeight="11232" activeTab="5" xr2:uid="{FEE1B7A2-A7F2-4786-A085-F6965BA5530A}"/>
   </bookViews>
   <sheets>
     <sheet name="LR" sheetId="1" r:id="rId1"/>
@@ -973,29 +973,29 @@
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="91.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="91.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>0.44400000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>0.44400000000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>20</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>0.44400000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>21</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>22</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>0.66100000000000003</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>23</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>24</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>0.57799999999999996</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>25</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>26</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>27</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>0.64800000000000002</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>28</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>29</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>30</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>31</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>32</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>34</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>0.66200000000000003</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>35</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>36</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>37</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>0.93400000000000005</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>38</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>39</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>0.93400000000000005</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>40</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>41</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>0.93400000000000005</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>42</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>43</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>44</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>45</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>46</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>47</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>48</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>49</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>50</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>0.93400000000000005</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>51</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>0.93400000000000005</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>52</v>
       </c>
@@ -1391,29 +1391,29 @@
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.90625" customWidth="1"/>
-    <col min="2" max="2" width="105.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="105.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>20</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>0.44400000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>21</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>22</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>23</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>24</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>25</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>26</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>27</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>28</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>29</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>30</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>31</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>32</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>34</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>35</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>36</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>55</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>56</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>57</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>58</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>59</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>60</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>61</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>62</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>63</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>64</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>65</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>66</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>67</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>68</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>69</v>
       </c>
@@ -1801,29 +1801,29 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.90625" customWidth="1"/>
-    <col min="2" max="2" width="180.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="180.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>0.93400000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>71</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>72</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>73</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>74</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>75</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>76</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>77</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>78</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>79</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>80</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>0.91700000000000004</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>81</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>82</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>83</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>84</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>85</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>86</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>87</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>88</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>89</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>90</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>0.93799999999999994</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>91</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>92</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>93</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>94</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>95</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>96</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>0.46300000000000002</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>97</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>0.93400000000000005</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>98</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>99</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>100</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>101</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>102</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>0.69199999999999995</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>103</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>0.92400000000000004</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>104</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>0.189</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>105</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>106</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>107</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>108</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>109</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>110</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>111</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>0.93799999999999994</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>112</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>113</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>114</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>115</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>116</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>117</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>118</v>
       </c>
@@ -2239,33 +2239,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B860205E-E1FC-4AF2-BCA5-2F337716C2FB}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="91.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="91.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>0.439</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>0.441</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0.443</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>20</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>119</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>120</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>121</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>0.44400000000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>122</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0.67100000000000004</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>123</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>0.61699999999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>124</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>125</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>126</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>0.68700000000000006</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>127</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>128</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>129</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>0.84399999999999997</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>130</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>131</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>0.752</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>132</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>133</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>0.754</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>134</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>0.86199999999999999</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>135</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>136</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>137</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>138</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>139</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>140</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>141</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>142</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>143</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>144</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>0.89100000000000001</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>145</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>146</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>147</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>148</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>184</v>
       </c>
@@ -2657,33 +2657,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B212AC66-1544-4FCE-ADF7-C01287B163F7}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
-    <col min="2" max="2" width="91.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="91.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>0.26200000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>0.10299999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>0.25800000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>0.439</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>0.25800000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0.443</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>0.26400000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>0.10299999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>0.104</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0.441</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>20</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>0.443</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>119</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>120</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>0.78500000000000003</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>121</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>0.44400000000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>122</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>0.77600000000000002</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>123</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>124</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>125</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>126</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>127</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>128</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>0.90100000000000002</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>129</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>130</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>131</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>0.78400000000000003</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>132</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>133</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>0.78600000000000003</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>134</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>0.91400000000000003</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>135</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>136</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>137</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>138</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>0.91100000000000003</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>139</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>0.90100000000000002</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>140</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>0.91300000000000003</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>141</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>142</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>143</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>144</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>145</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>0.82599999999999996</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>146</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>147</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>0.91400000000000003</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>148</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>185</v>
       </c>
@@ -3075,33 +3075,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2315BCA-BE68-41F1-B1B5-A704F37DD4B4}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" customWidth="1"/>
-    <col min="2" max="2" width="93.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="93.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>20</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>0.85599999999999998</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>154</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>155</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>0.90800000000000003</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>156</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>157</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>158</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>159</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>160</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>161</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>0.91100000000000003</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>162</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>163</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>0.94199999999999995</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>164</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>165</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>166</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>167</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>168</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>169</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>170</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>0.95599999999999996</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>171</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>172</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>0.94199999999999995</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>173</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>0.95699999999999996</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>174</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>175</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>176</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>0.95699999999999996</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>177</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>0.94499999999999995</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>178</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>179</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>0.95399999999999996</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>180</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>181</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>0.95599999999999996</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>182</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>183</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>186</v>
       </c>

</xml_diff>